<commit_message>
Including setbacks in archetypes
</commit_message>
<xml_diff>
--- a/cea/db/Archetypes/Switzerland/Archetypes_properties.xlsx
+++ b/cea/db/Archetypes/Switzerland/Archetypes_properties.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" tabRatio="785" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" tabRatio="785" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3728" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3730" uniqueCount="273">
   <si>
     <t>Code</t>
   </si>
@@ -838,6 +838,12 @@
   </si>
   <si>
     <t>Ed_Wm2</t>
+  </si>
+  <si>
+    <t>Tcs_setb_C</t>
+  </si>
+  <si>
+    <t>Ths_setb_C</t>
   </si>
 </sst>
 </file>
@@ -5395,7 +5401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A43" sqref="A43:XFD50"/>
     </sheetView>
   </sheetViews>
@@ -15400,10 +15406,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:A16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15411,11 +15417,13 @@
     <col min="1" max="1" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -15426,10 +15434,16 @@
         <v>220</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>230</v>
       </c>
@@ -15439,11 +15453,17 @@
       <c r="C2" s="11">
         <v>22</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="3">
+        <v>28</v>
+      </c>
+      <c r="E2" s="10">
+        <v>18</v>
+      </c>
+      <c r="F2" s="11">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>231</v>
       </c>
@@ -15453,11 +15473,17 @@
       <c r="C3" s="11">
         <v>22</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="3">
+        <v>28</v>
+      </c>
+      <c r="E3" s="10">
+        <v>18</v>
+      </c>
+      <c r="F3" s="11">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>232</v>
       </c>
@@ -15467,11 +15493,17 @@
       <c r="C4" s="15">
         <v>21</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="3">
+        <v>28</v>
+      </c>
+      <c r="E4" s="10">
+        <v>21</v>
+      </c>
+      <c r="F4" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>233</v>
       </c>
@@ -15481,11 +15513,17 @@
       <c r="C5" s="15">
         <v>22</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="3">
+        <v>28</v>
+      </c>
+      <c r="E5" s="10">
+        <v>12</v>
+      </c>
+      <c r="F5" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>234</v>
       </c>
@@ -15495,11 +15533,17 @@
       <c r="C6" s="15">
         <v>20</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="3">
+        <v>28</v>
+      </c>
+      <c r="E6" s="10">
+        <v>12</v>
+      </c>
+      <c r="F6" s="15">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>244</v>
       </c>
@@ -15509,11 +15553,17 @@
       <c r="C7" s="15">
         <v>22</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="3">
+        <v>28</v>
+      </c>
+      <c r="E7" s="10">
+        <v>12</v>
+      </c>
+      <c r="F7" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>235</v>
       </c>
@@ -15523,12 +15573,18 @@
       <c r="C8" s="15">
         <v>21</v>
       </c>
-      <c r="D8" s="15">
-        <f t="shared" ref="D8" si="0">111*0.15+10*0.85</f>
+      <c r="D8" s="3">
+        <v>28</v>
+      </c>
+      <c r="E8" s="10">
+        <v>12</v>
+      </c>
+      <c r="F8" s="15">
+        <f t="shared" ref="F8" si="0">111*0.15+10*0.85</f>
         <v>25.15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>236</v>
       </c>
@@ -15538,11 +15594,17 @@
       <c r="C9" s="15">
         <v>21</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="3">
+        <v>28</v>
+      </c>
+      <c r="E9" s="10">
+        <v>12</v>
+      </c>
+      <c r="F9" s="15">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>237</v>
       </c>
@@ -15552,11 +15614,17 @@
       <c r="C10" s="15">
         <v>21</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="3">
+        <v>28</v>
+      </c>
+      <c r="E10" s="10">
+        <v>12</v>
+      </c>
+      <c r="F10" s="15">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>238</v>
       </c>
@@ -15566,11 +15634,17 @@
       <c r="C11" s="15">
         <v>22</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="3">
+        <v>28</v>
+      </c>
+      <c r="E11" s="10">
+        <v>21</v>
+      </c>
+      <c r="F11" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>239</v>
       </c>
@@ -15580,11 +15654,17 @@
       <c r="C12" s="15">
         <v>18</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="3">
+        <v>28</v>
+      </c>
+      <c r="E12" s="10">
+        <v>12</v>
+      </c>
+      <c r="F12" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>240</v>
       </c>
@@ -15594,11 +15674,17 @@
       <c r="C13" s="15">
         <v>24</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="3">
+        <v>28</v>
+      </c>
+      <c r="E13" s="10">
+        <v>12</v>
+      </c>
+      <c r="F13" s="15">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>241</v>
       </c>
@@ -15608,11 +15694,17 @@
       <c r="C14" s="15">
         <v>26</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="3">
+        <v>28</v>
+      </c>
+      <c r="E14" s="10">
+        <v>12</v>
+      </c>
+      <c r="F14" s="15">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>242</v>
       </c>
@@ -15622,11 +15714,17 @@
       <c r="C15" s="15">
         <v>18</v>
       </c>
-      <c r="D15" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="3">
+        <v>28</v>
+      </c>
+      <c r="E15" s="10">
+        <v>12</v>
+      </c>
+      <c r="F15" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>243</v>
       </c>
@@ -15636,7 +15734,13 @@
       <c r="C16" s="15">
         <v>-5</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="3">
+        <v>28</v>
+      </c>
+      <c r="E16" s="10">
+        <v>-5</v>
+      </c>
+      <c r="F16" s="15">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ventilation properties in archetypes db
</commit_message>
<xml_diff>
--- a/cea/db/Archetypes/Switzerland/Archetypes_properties.xlsx
+++ b/cea/db/Archetypes/Switzerland/Archetypes_properties.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JF\Documents\CEAforArcGIS\cea\db\Archetypes\Switzerland\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fcl2\AppData\Roaming\ESRI\Desktop10.3\ArcToolbox\My Toolboxes\cea\db\Archetypes\Switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" tabRatio="785" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" tabRatio="785"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <sheet name="EMBODIED_ENERGY" sheetId="5" r:id="rId6"/>
     <sheet name="EMBODIED_EMISSIONS" sheetId="4" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3730" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3732" uniqueCount="275">
   <si>
     <t>Code</t>
   </si>
@@ -845,11 +845,17 @@
   <si>
     <t>Ths_setb_C</t>
   </si>
+  <si>
+    <t>n50</t>
+  </si>
+  <si>
+    <t>win_op</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1370,7 +1376,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1420,6 +1426,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1742,10 +1751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F181"/>
+  <dimension ref="A1:H181"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F1" sqref="B1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,11 +1764,11 @@
     <col min="3" max="3" width="12.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="4" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1778,8 +1787,14 @@
       <c r="F1" s="13" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -1798,8 +1813,14 @@
       <c r="F2" s="10">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="11">
+        <v>3</v>
+      </c>
+      <c r="H2" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>30</v>
       </c>
@@ -1818,8 +1839,14 @@
       <c r="F3" s="10">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="11">
+        <v>3</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>31</v>
       </c>
@@ -1838,8 +1865,14 @@
       <c r="F4" s="10">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="11">
+        <v>3</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>32</v>
       </c>
@@ -1858,8 +1891,14 @@
       <c r="F5" s="10">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="11">
+        <v>3</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>33</v>
       </c>
@@ -1878,8 +1917,14 @@
       <c r="F6" s="10">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="11">
+        <v>2</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>34</v>
       </c>
@@ -1898,8 +1943,14 @@
       <c r="F7" s="10">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="11">
+        <v>1</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>35</v>
       </c>
@@ -1918,8 +1969,14 @@
       <c r="F8" s="10">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="11">
+        <v>2</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>36</v>
       </c>
@@ -1938,8 +1995,14 @@
       <c r="F9" s="10">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="11">
+        <v>2</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>37</v>
       </c>
@@ -1958,8 +2021,14 @@
       <c r="F10" s="10">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="11">
+        <v>2</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>38</v>
       </c>
@@ -1978,8 +2047,14 @@
       <c r="F11" s="10">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="11">
+        <v>2</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>39</v>
       </c>
@@ -1998,8 +2073,14 @@
       <c r="F12" s="10">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="11">
+        <v>2</v>
+      </c>
+      <c r="H12" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>40</v>
       </c>
@@ -2018,8 +2099,14 @@
       <c r="F13" s="10">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="11">
+        <v>1</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>53</v>
       </c>
@@ -2038,8 +2125,14 @@
       <c r="F14" s="10">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="11">
+        <v>3</v>
+      </c>
+      <c r="H14" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>54</v>
       </c>
@@ -2058,8 +2151,14 @@
       <c r="F15" s="10">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="11">
+        <v>3</v>
+      </c>
+      <c r="H15" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>55</v>
       </c>
@@ -2078,8 +2177,14 @@
       <c r="F16" s="10">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="11">
+        <v>3</v>
+      </c>
+      <c r="H16" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>56</v>
       </c>
@@ -2098,8 +2203,14 @@
       <c r="F17" s="10">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="11">
+        <v>3</v>
+      </c>
+      <c r="H17" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>57</v>
       </c>
@@ -2118,8 +2229,14 @@
       <c r="F18" s="10">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="11">
+        <v>2</v>
+      </c>
+      <c r="H18" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>58</v>
       </c>
@@ -2138,8 +2255,14 @@
       <c r="F19" s="10">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="11">
+        <v>1</v>
+      </c>
+      <c r="H19" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>59</v>
       </c>
@@ -2158,8 +2281,14 @@
       <c r="F20" s="10">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="11">
+        <v>2</v>
+      </c>
+      <c r="H20" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>60</v>
       </c>
@@ -2178,8 +2307,14 @@
       <c r="F21" s="10">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="11">
+        <v>2</v>
+      </c>
+      <c r="H21" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>61</v>
       </c>
@@ -2198,8 +2333,14 @@
       <c r="F22" s="10">
         <v>60</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="11">
+        <v>2</v>
+      </c>
+      <c r="H22" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>62</v>
       </c>
@@ -2218,8 +2359,14 @@
       <c r="F23" s="10">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="11">
+        <v>2</v>
+      </c>
+      <c r="H23" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>63</v>
       </c>
@@ -2238,8 +2385,14 @@
       <c r="F24" s="10">
         <v>60</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="11">
+        <v>2</v>
+      </c>
+      <c r="H24" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>64</v>
       </c>
@@ -2258,8 +2411,14 @@
       <c r="F25" s="10">
         <v>60</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="11">
+        <v>1</v>
+      </c>
+      <c r="H25" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>41</v>
       </c>
@@ -2279,8 +2438,14 @@
         <f>10*0.9+0.1*5</f>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="18">
+        <v>6</v>
+      </c>
+      <c r="H26" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>42</v>
       </c>
@@ -2300,8 +2465,14 @@
         <f t="shared" ref="F27:F37" si="0">10*0.9+0.1*5</f>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="18">
+        <v>6</v>
+      </c>
+      <c r="H27" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>43</v>
       </c>
@@ -2321,8 +2492,14 @@
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="18">
+        <v>6</v>
+      </c>
+      <c r="H28" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>44</v>
       </c>
@@ -2342,8 +2519,14 @@
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="18">
+        <v>4</v>
+      </c>
+      <c r="H29" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>45</v>
       </c>
@@ -2363,8 +2546,14 @@
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="18">
+        <v>2</v>
+      </c>
+      <c r="H30" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>46</v>
       </c>
@@ -2384,8 +2573,14 @@
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="18">
+        <v>1</v>
+      </c>
+      <c r="H31" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>47</v>
       </c>
@@ -2405,8 +2600,14 @@
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="18">
+        <v>2</v>
+      </c>
+      <c r="H32" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>48</v>
       </c>
@@ -2426,8 +2627,14 @@
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="18">
+        <v>2</v>
+      </c>
+      <c r="H33" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>49</v>
       </c>
@@ -2447,8 +2654,14 @@
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="18">
+        <v>2</v>
+      </c>
+      <c r="H34" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>50</v>
       </c>
@@ -2468,8 +2681,14 @@
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="18">
+        <v>2</v>
+      </c>
+      <c r="H35" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>51</v>
       </c>
@@ -2489,8 +2708,14 @@
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="18">
+        <v>2</v>
+      </c>
+      <c r="H36" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>52</v>
       </c>
@@ -2510,8 +2735,14 @@
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="18">
+        <v>1</v>
+      </c>
+      <c r="H37" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>65</v>
       </c>
@@ -2530,8 +2761,14 @@
       <c r="F38" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="15">
+        <v>6</v>
+      </c>
+      <c r="H38" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>66</v>
       </c>
@@ -2550,8 +2787,14 @@
       <c r="F39" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="15">
+        <v>6</v>
+      </c>
+      <c r="H39" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>67</v>
       </c>
@@ -2570,8 +2813,14 @@
       <c r="F40" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="15">
+        <v>6</v>
+      </c>
+      <c r="H40" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>68</v>
       </c>
@@ -2590,8 +2839,14 @@
       <c r="F41" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="15">
+        <v>6</v>
+      </c>
+      <c r="H41" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>69</v>
       </c>
@@ -2610,8 +2865,14 @@
       <c r="F42" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="15">
+        <v>2</v>
+      </c>
+      <c r="H42" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>70</v>
       </c>
@@ -2630,8 +2891,14 @@
       <c r="F43" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="15">
+        <v>1</v>
+      </c>
+      <c r="H43" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>71</v>
       </c>
@@ -2650,8 +2917,14 @@
       <c r="F44" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="15">
+        <v>2</v>
+      </c>
+      <c r="H44" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>72</v>
       </c>
@@ -2670,8 +2943,14 @@
       <c r="F45" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="15">
+        <v>2</v>
+      </c>
+      <c r="H45" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>73</v>
       </c>
@@ -2690,8 +2969,14 @@
       <c r="F46" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="15">
+        <v>2</v>
+      </c>
+      <c r="H46" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>74</v>
       </c>
@@ -2710,8 +2995,14 @@
       <c r="F47" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" s="15">
+        <v>2</v>
+      </c>
+      <c r="H47" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>75</v>
       </c>
@@ -2730,8 +3021,14 @@
       <c r="F48" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="15">
+        <v>2</v>
+      </c>
+      <c r="H48" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>76</v>
       </c>
@@ -2750,8 +3047,14 @@
       <c r="F49" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="15">
+        <v>1</v>
+      </c>
+      <c r="H49" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>77</v>
       </c>
@@ -2770,8 +3073,14 @@
       <c r="F50" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="15">
+        <v>6</v>
+      </c>
+      <c r="H50" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>78</v>
       </c>
@@ -2790,8 +3099,14 @@
       <c r="F51" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="15">
+        <v>6</v>
+      </c>
+      <c r="H51" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
         <v>79</v>
       </c>
@@ -2810,8 +3125,14 @@
       <c r="F52" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" s="15">
+        <v>6</v>
+      </c>
+      <c r="H52" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>80</v>
       </c>
@@ -2830,8 +3151,14 @@
       <c r="F53" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" s="15">
+        <v>6</v>
+      </c>
+      <c r="H53" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>81</v>
       </c>
@@ -2850,8 +3177,14 @@
       <c r="F54" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" s="15">
+        <v>2</v>
+      </c>
+      <c r="H54" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>82</v>
       </c>
@@ -2870,8 +3203,14 @@
       <c r="F55" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55" s="15">
+        <v>1</v>
+      </c>
+      <c r="H55" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>83</v>
       </c>
@@ -2890,8 +3229,14 @@
       <c r="F56" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" s="15">
+        <v>2</v>
+      </c>
+      <c r="H56" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>84</v>
       </c>
@@ -2910,8 +3255,14 @@
       <c r="F57" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57" s="15">
+        <v>2</v>
+      </c>
+      <c r="H57" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>85</v>
       </c>
@@ -2930,8 +3281,14 @@
       <c r="F58" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58" s="15">
+        <v>2</v>
+      </c>
+      <c r="H58" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
         <v>86</v>
       </c>
@@ -2950,8 +3307,14 @@
       <c r="F59" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59" s="15">
+        <v>2</v>
+      </c>
+      <c r="H59" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
         <v>87</v>
       </c>
@@ -2970,8 +3333,14 @@
       <c r="F60" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60" s="15">
+        <v>2</v>
+      </c>
+      <c r="H60" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>88</v>
       </c>
@@ -2990,8 +3359,14 @@
       <c r="F61" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61" s="15">
+        <v>1</v>
+      </c>
+      <c r="H61" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>245</v>
       </c>
@@ -3010,8 +3385,14 @@
       <c r="F62" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62" s="15">
+        <v>6</v>
+      </c>
+      <c r="H62" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>246</v>
       </c>
@@ -3030,8 +3411,14 @@
       <c r="F63" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63" s="15">
+        <v>6</v>
+      </c>
+      <c r="H63" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>247</v>
       </c>
@@ -3050,8 +3437,14 @@
       <c r="F64" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64" s="15">
+        <v>6</v>
+      </c>
+      <c r="H64" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
         <v>248</v>
       </c>
@@ -3070,8 +3463,14 @@
       <c r="F65" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65" s="15">
+        <v>6</v>
+      </c>
+      <c r="H65" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>249</v>
       </c>
@@ -3090,8 +3489,14 @@
       <c r="F66" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66" s="15">
+        <v>2</v>
+      </c>
+      <c r="H66" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>250</v>
       </c>
@@ -3110,8 +3515,14 @@
       <c r="F67" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G67" s="15">
+        <v>1</v>
+      </c>
+      <c r="H67" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
         <v>251</v>
       </c>
@@ -3130,8 +3541,14 @@
       <c r="F68" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68" s="15">
+        <v>2</v>
+      </c>
+      <c r="H68" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
         <v>252</v>
       </c>
@@ -3150,8 +3567,14 @@
       <c r="F69" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69" s="15">
+        <v>2</v>
+      </c>
+      <c r="H69" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
         <v>253</v>
       </c>
@@ -3170,8 +3593,14 @@
       <c r="F70" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70" s="15">
+        <v>2</v>
+      </c>
+      <c r="H70" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
         <v>254</v>
       </c>
@@ -3190,8 +3619,14 @@
       <c r="F71" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G71" s="15">
+        <v>2</v>
+      </c>
+      <c r="H71" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
         <v>255</v>
       </c>
@@ -3210,8 +3645,14 @@
       <c r="F72" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G72" s="15">
+        <v>2</v>
+      </c>
+      <c r="H72" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
         <v>256</v>
       </c>
@@ -3230,8 +3671,14 @@
       <c r="F73" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G73" s="15">
+        <v>1</v>
+      </c>
+      <c r="H73" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
         <v>101</v>
       </c>
@@ -3250,8 +3697,14 @@
       <c r="F74" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74" s="15">
+        <v>6</v>
+      </c>
+      <c r="H74" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
         <v>102</v>
       </c>
@@ -3270,8 +3723,14 @@
       <c r="F75" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75" s="15">
+        <v>6</v>
+      </c>
+      <c r="H75" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
         <v>103</v>
       </c>
@@ -3290,8 +3749,14 @@
       <c r="F76" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76" s="15">
+        <v>6</v>
+      </c>
+      <c r="H76" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
         <v>104</v>
       </c>
@@ -3310,8 +3775,14 @@
       <c r="F77" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77" s="15">
+        <v>6</v>
+      </c>
+      <c r="H77" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
         <v>105</v>
       </c>
@@ -3330,8 +3801,14 @@
       <c r="F78" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78" s="15">
+        <v>2</v>
+      </c>
+      <c r="H78" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
         <v>106</v>
       </c>
@@ -3350,8 +3827,14 @@
       <c r="F79" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79" s="15">
+        <v>1</v>
+      </c>
+      <c r="H79" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>107</v>
       </c>
@@ -3370,8 +3853,14 @@
       <c r="F80" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80" s="15">
+        <v>2</v>
+      </c>
+      <c r="H80" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
         <v>108</v>
       </c>
@@ -3390,8 +3879,14 @@
       <c r="F81" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G81" s="15">
+        <v>2</v>
+      </c>
+      <c r="H81" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
         <v>109</v>
       </c>
@@ -3410,8 +3905,14 @@
       <c r="F82" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82" s="15">
+        <v>2</v>
+      </c>
+      <c r="H82" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
         <v>110</v>
       </c>
@@ -3430,8 +3931,14 @@
       <c r="F83" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G83" s="15">
+        <v>2</v>
+      </c>
+      <c r="H83" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
         <v>111</v>
       </c>
@@ -3450,8 +3957,14 @@
       <c r="F84" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G84" s="15">
+        <v>2</v>
+      </c>
+      <c r="H84" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
         <v>112</v>
       </c>
@@ -3470,8 +3983,14 @@
       <c r="F85" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G85" s="15">
+        <v>1</v>
+      </c>
+      <c r="H85" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
         <v>113</v>
       </c>
@@ -3490,8 +4009,14 @@
       <c r="F86" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G86" s="15">
+        <v>6</v>
+      </c>
+      <c r="H86" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>114</v>
       </c>
@@ -3510,8 +4035,14 @@
       <c r="F87" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G87" s="15">
+        <v>6</v>
+      </c>
+      <c r="H87" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>115</v>
       </c>
@@ -3530,8 +4061,14 @@
       <c r="F88" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G88" s="15">
+        <v>6</v>
+      </c>
+      <c r="H88" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
         <v>116</v>
       </c>
@@ -3550,8 +4087,14 @@
       <c r="F89" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G89" s="15">
+        <v>4</v>
+      </c>
+      <c r="H89" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
         <v>117</v>
       </c>
@@ -3570,8 +4113,14 @@
       <c r="F90" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G90" s="15">
+        <v>2</v>
+      </c>
+      <c r="H90" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
         <v>118</v>
       </c>
@@ -3590,8 +4139,14 @@
       <c r="F91" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G91" s="15">
+        <v>1</v>
+      </c>
+      <c r="H91" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>119</v>
       </c>
@@ -3610,8 +4165,14 @@
       <c r="F92" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G92" s="15">
+        <v>2</v>
+      </c>
+      <c r="H92" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
         <v>120</v>
       </c>
@@ -3630,8 +4191,14 @@
       <c r="F93" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G93" s="15">
+        <v>2</v>
+      </c>
+      <c r="H93" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
         <v>121</v>
       </c>
@@ -3650,8 +4217,14 @@
       <c r="F94" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G94" s="15">
+        <v>2</v>
+      </c>
+      <c r="H94" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
         <v>122</v>
       </c>
@@ -3670,8 +4243,14 @@
       <c r="F95" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G95" s="15">
+        <v>2</v>
+      </c>
+      <c r="H95" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
         <v>123</v>
       </c>
@@ -3690,8 +4269,14 @@
       <c r="F96" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G96" s="15">
+        <v>2</v>
+      </c>
+      <c r="H96" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
         <v>124</v>
       </c>
@@ -3710,8 +4295,14 @@
       <c r="F97" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G97" s="15">
+        <v>1</v>
+      </c>
+      <c r="H97" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
         <v>125</v>
       </c>
@@ -3730,8 +4321,14 @@
       <c r="F98" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G98" s="15">
+        <v>6</v>
+      </c>
+      <c r="H98" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
         <v>126</v>
       </c>
@@ -3750,8 +4347,14 @@
       <c r="F99" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G99" s="15">
+        <v>6</v>
+      </c>
+      <c r="H99" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
         <v>127</v>
       </c>
@@ -3770,8 +4373,14 @@
       <c r="F100" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G100" s="15">
+        <v>6</v>
+      </c>
+      <c r="H100" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
         <v>128</v>
       </c>
@@ -3790,8 +4399,14 @@
       <c r="F101" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G101" s="15">
+        <v>4</v>
+      </c>
+      <c r="H101" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
         <v>129</v>
       </c>
@@ -3810,8 +4425,14 @@
       <c r="F102" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G102" s="15">
+        <v>2</v>
+      </c>
+      <c r="H102" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
         <v>130</v>
       </c>
@@ -3830,8 +4451,14 @@
       <c r="F103" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G103" s="15">
+        <v>1</v>
+      </c>
+      <c r="H103" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
         <v>131</v>
       </c>
@@ -3850,8 +4477,14 @@
       <c r="F104" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G104" s="15">
+        <v>2</v>
+      </c>
+      <c r="H104" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
         <v>132</v>
       </c>
@@ -3870,8 +4503,14 @@
       <c r="F105" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G105" s="15">
+        <v>2</v>
+      </c>
+      <c r="H105" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
         <v>133</v>
       </c>
@@ -3890,8 +4529,14 @@
       <c r="F106" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G106" s="15">
+        <v>2</v>
+      </c>
+      <c r="H106" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
         <v>134</v>
       </c>
@@ -3910,8 +4555,14 @@
       <c r="F107" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G107" s="15">
+        <v>2</v>
+      </c>
+      <c r="H107" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
         <v>135</v>
       </c>
@@ -3930,8 +4581,14 @@
       <c r="F108" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G108" s="15">
+        <v>2</v>
+      </c>
+      <c r="H108" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
         <v>136</v>
       </c>
@@ -3950,8 +4607,14 @@
       <c r="F109" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G109" s="15">
+        <v>1</v>
+      </c>
+      <c r="H109" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="s">
         <v>137</v>
       </c>
@@ -3970,8 +4633,14 @@
       <c r="F110" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G110" s="15">
+        <v>6</v>
+      </c>
+      <c r="H110" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="s">
         <v>138</v>
       </c>
@@ -3990,8 +4659,14 @@
       <c r="F111" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G111" s="15">
+        <v>6</v>
+      </c>
+      <c r="H111" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
         <v>139</v>
       </c>
@@ -4010,8 +4685,14 @@
       <c r="F112" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G112" s="15">
+        <v>6</v>
+      </c>
+      <c r="H112" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
         <v>140</v>
       </c>
@@ -4030,8 +4711,14 @@
       <c r="F113" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G113" s="15">
+        <v>4</v>
+      </c>
+      <c r="H113" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="13" t="s">
         <v>141</v>
       </c>
@@ -4050,8 +4737,14 @@
       <c r="F114" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G114" s="15">
+        <v>2</v>
+      </c>
+      <c r="H114" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="13" t="s">
         <v>142</v>
       </c>
@@ -4070,8 +4763,14 @@
       <c r="F115" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G115" s="15">
+        <v>1</v>
+      </c>
+      <c r="H115" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="13" t="s">
         <v>143</v>
       </c>
@@ -4090,8 +4789,14 @@
       <c r="F116" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G116" s="15">
+        <v>2</v>
+      </c>
+      <c r="H116" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
         <v>144</v>
       </c>
@@ -4110,8 +4815,14 @@
       <c r="F117" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G117" s="15">
+        <v>2</v>
+      </c>
+      <c r="H117" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
         <v>145</v>
       </c>
@@ -4130,8 +4841,14 @@
       <c r="F118" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G118" s="15">
+        <v>2</v>
+      </c>
+      <c r="H118" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
         <v>146</v>
       </c>
@@ -4150,8 +4867,14 @@
       <c r="F119" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G119" s="15">
+        <v>2</v>
+      </c>
+      <c r="H119" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
         <v>147</v>
       </c>
@@ -4170,8 +4893,14 @@
       <c r="F120" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G120" s="15">
+        <v>2</v>
+      </c>
+      <c r="H120" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="s">
         <v>148</v>
       </c>
@@ -4190,8 +4919,14 @@
       <c r="F121" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G121" s="15">
+        <v>1</v>
+      </c>
+      <c r="H121" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="13" t="s">
         <v>149</v>
       </c>
@@ -4210,8 +4945,14 @@
       <c r="F122" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G122" s="15">
+        <v>6</v>
+      </c>
+      <c r="H122" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="13" t="s">
         <v>150</v>
       </c>
@@ -4230,8 +4971,14 @@
       <c r="F123" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G123" s="15">
+        <v>6</v>
+      </c>
+      <c r="H123" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="s">
         <v>151</v>
       </c>
@@ -4250,8 +4997,14 @@
       <c r="F124" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G124" s="15">
+        <v>6</v>
+      </c>
+      <c r="H124" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="13" t="s">
         <v>152</v>
       </c>
@@ -4270,8 +5023,14 @@
       <c r="F125" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G125" s="15">
+        <v>4</v>
+      </c>
+      <c r="H125" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="13" t="s">
         <v>153</v>
       </c>
@@ -4290,8 +5049,14 @@
       <c r="F126" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G126" s="15">
+        <v>2</v>
+      </c>
+      <c r="H126" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="13" t="s">
         <v>154</v>
       </c>
@@ -4310,8 +5075,14 @@
       <c r="F127" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G127" s="15">
+        <v>1</v>
+      </c>
+      <c r="H127" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="13" t="s">
         <v>155</v>
       </c>
@@ -4330,8 +5101,14 @@
       <c r="F128" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G128" s="15">
+        <v>2</v>
+      </c>
+      <c r="H128" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="13" t="s">
         <v>156</v>
       </c>
@@ -4350,8 +5127,14 @@
       <c r="F129" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G129" s="15">
+        <v>2</v>
+      </c>
+      <c r="H129" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="13" t="s">
         <v>157</v>
       </c>
@@ -4370,8 +5153,14 @@
       <c r="F130" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G130" s="15">
+        <v>2</v>
+      </c>
+      <c r="H130" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="13" t="s">
         <v>158</v>
       </c>
@@ -4390,8 +5179,14 @@
       <c r="F131" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G131" s="15">
+        <v>2</v>
+      </c>
+      <c r="H131" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="13" t="s">
         <v>159</v>
       </c>
@@ -4410,8 +5205,14 @@
       <c r="F132" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G132" s="15">
+        <v>2</v>
+      </c>
+      <c r="H132" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
         <v>160</v>
       </c>
@@ -4430,8 +5231,14 @@
       <c r="F133" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G133" s="15">
+        <v>1</v>
+      </c>
+      <c r="H133" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="13" t="s">
         <v>161</v>
       </c>
@@ -4450,8 +5257,14 @@
       <c r="F134" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G134" s="15">
+        <v>6</v>
+      </c>
+      <c r="H134" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="13" t="s">
         <v>162</v>
       </c>
@@ -4470,8 +5283,14 @@
       <c r="F135" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G135" s="15">
+        <v>6</v>
+      </c>
+      <c r="H135" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="13" t="s">
         <v>163</v>
       </c>
@@ -4490,8 +5309,14 @@
       <c r="F136" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G136" s="15">
+        <v>6</v>
+      </c>
+      <c r="H136" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="13" t="s">
         <v>164</v>
       </c>
@@ -4510,8 +5335,14 @@
       <c r="F137" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G137" s="15">
+        <v>4</v>
+      </c>
+      <c r="H137" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="13" t="s">
         <v>165</v>
       </c>
@@ -4530,8 +5361,14 @@
       <c r="F138" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G138" s="15">
+        <v>2</v>
+      </c>
+      <c r="H138" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="13" t="s">
         <v>166</v>
       </c>
@@ -4550,8 +5387,14 @@
       <c r="F139" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G139" s="15">
+        <v>1</v>
+      </c>
+      <c r="H139" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="13" t="s">
         <v>167</v>
       </c>
@@ -4570,8 +5413,14 @@
       <c r="F140" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G140" s="15">
+        <v>2</v>
+      </c>
+      <c r="H140" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="13" t="s">
         <v>168</v>
       </c>
@@ -4590,8 +5439,14 @@
       <c r="F141" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G141" s="15">
+        <v>2</v>
+      </c>
+      <c r="H141" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="13" t="s">
         <v>169</v>
       </c>
@@ -4610,8 +5465,14 @@
       <c r="F142" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G142" s="15">
+        <v>2</v>
+      </c>
+      <c r="H142" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="13" t="s">
         <v>170</v>
       </c>
@@ -4630,8 +5491,14 @@
       <c r="F143" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G143" s="15">
+        <v>2</v>
+      </c>
+      <c r="H143" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="13" t="s">
         <v>171</v>
       </c>
@@ -4650,8 +5517,14 @@
       <c r="F144" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G144" s="15">
+        <v>2</v>
+      </c>
+      <c r="H144" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
         <v>172</v>
       </c>
@@ -4670,8 +5543,14 @@
       <c r="F145" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G145" s="15">
+        <v>1</v>
+      </c>
+      <c r="H145" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="13" t="s">
         <v>173</v>
       </c>
@@ -4690,8 +5569,14 @@
       <c r="F146" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G146" s="15">
+        <v>6</v>
+      </c>
+      <c r="H146" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="13" t="s">
         <v>174</v>
       </c>
@@ -4710,8 +5595,14 @@
       <c r="F147" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G147" s="15">
+        <v>6</v>
+      </c>
+      <c r="H147" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="13" t="s">
         <v>175</v>
       </c>
@@ -4730,8 +5621,14 @@
       <c r="F148" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G148" s="15">
+        <v>6</v>
+      </c>
+      <c r="H148" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="13" t="s">
         <v>176</v>
       </c>
@@ -4750,8 +5647,14 @@
       <c r="F149" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G149" s="15">
+        <v>4</v>
+      </c>
+      <c r="H149" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="13" t="s">
         <v>177</v>
       </c>
@@ -4770,8 +5673,14 @@
       <c r="F150" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G150" s="15">
+        <v>2</v>
+      </c>
+      <c r="H150" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="13" t="s">
         <v>178</v>
       </c>
@@ -4790,8 +5699,14 @@
       <c r="F151" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G151" s="15">
+        <v>1</v>
+      </c>
+      <c r="H151" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="13" t="s">
         <v>179</v>
       </c>
@@ -4810,8 +5725,14 @@
       <c r="F152" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G152" s="15">
+        <v>2</v>
+      </c>
+      <c r="H152" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="13" t="s">
         <v>180</v>
       </c>
@@ -4830,8 +5751,14 @@
       <c r="F153" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G153" s="15">
+        <v>2</v>
+      </c>
+      <c r="H153" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="13" t="s">
         <v>181</v>
       </c>
@@ -4850,8 +5777,14 @@
       <c r="F154" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G154" s="15">
+        <v>2</v>
+      </c>
+      <c r="H154" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="13" t="s">
         <v>182</v>
       </c>
@@ -4870,8 +5803,14 @@
       <c r="F155" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G155" s="15">
+        <v>2</v>
+      </c>
+      <c r="H155" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="13" t="s">
         <v>183</v>
       </c>
@@ -4890,8 +5829,14 @@
       <c r="F156" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G156" s="15">
+        <v>2</v>
+      </c>
+      <c r="H156" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="13" t="s">
         <v>184</v>
       </c>
@@ -4910,8 +5855,14 @@
       <c r="F157" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G157" s="15">
+        <v>1</v>
+      </c>
+      <c r="H157" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="13" t="s">
         <v>185</v>
       </c>
@@ -4930,8 +5881,14 @@
       <c r="F158" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G158" s="15">
+        <v>6</v>
+      </c>
+      <c r="H158" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="13" t="s">
         <v>186</v>
       </c>
@@ -4950,8 +5907,14 @@
       <c r="F159" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G159" s="15">
+        <v>6</v>
+      </c>
+      <c r="H159" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="13" t="s">
         <v>187</v>
       </c>
@@ -4970,8 +5933,14 @@
       <c r="F160" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G160" s="15">
+        <v>6</v>
+      </c>
+      <c r="H160" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="13" t="s">
         <v>188</v>
       </c>
@@ -4990,8 +5959,14 @@
       <c r="F161" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G161" s="15">
+        <v>6</v>
+      </c>
+      <c r="H161" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="13" t="s">
         <v>189</v>
       </c>
@@ -5010,8 +5985,14 @@
       <c r="F162" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G162" s="15">
+        <v>2</v>
+      </c>
+      <c r="H162" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="13" t="s">
         <v>190</v>
       </c>
@@ -5030,8 +6011,14 @@
       <c r="F163" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G163" s="15">
+        <v>1</v>
+      </c>
+      <c r="H163" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="13" t="s">
         <v>191</v>
       </c>
@@ -5050,8 +6037,14 @@
       <c r="F164" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G164" s="15">
+        <v>2</v>
+      </c>
+      <c r="H164" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="13" t="s">
         <v>192</v>
       </c>
@@ -5070,8 +6063,14 @@
       <c r="F165" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G165" s="15">
+        <v>2</v>
+      </c>
+      <c r="H165" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="13" t="s">
         <v>193</v>
       </c>
@@ -5090,8 +6089,14 @@
       <c r="F166" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G166" s="15">
+        <v>2</v>
+      </c>
+      <c r="H166" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="13" t="s">
         <v>194</v>
       </c>
@@ -5110,8 +6115,14 @@
       <c r="F167" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G167" s="15">
+        <v>2</v>
+      </c>
+      <c r="H167" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="13" t="s">
         <v>195</v>
       </c>
@@ -5130,8 +6141,14 @@
       <c r="F168" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G168" s="15">
+        <v>2</v>
+      </c>
+      <c r="H168" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="13" t="s">
         <v>196</v>
       </c>
@@ -5150,8 +6167,14 @@
       <c r="F169" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G169" s="15">
+        <v>1</v>
+      </c>
+      <c r="H169" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="13" t="s">
         <v>197</v>
       </c>
@@ -5170,8 +6193,14 @@
       <c r="F170" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G170" s="15">
+        <v>6</v>
+      </c>
+      <c r="H170" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="13" t="s">
         <v>198</v>
       </c>
@@ -5190,8 +6219,14 @@
       <c r="F171" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G171" s="15">
+        <v>6</v>
+      </c>
+      <c r="H171" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="13" t="s">
         <v>199</v>
       </c>
@@ -5210,8 +6245,14 @@
       <c r="F172" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G172" s="15">
+        <v>6</v>
+      </c>
+      <c r="H172" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="13" t="s">
         <v>200</v>
       </c>
@@ -5230,8 +6271,14 @@
       <c r="F173" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G173" s="15">
+        <v>4</v>
+      </c>
+      <c r="H173" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="13" t="s">
         <v>201</v>
       </c>
@@ -5250,8 +6297,14 @@
       <c r="F174" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G174" s="15">
+        <v>2</v>
+      </c>
+      <c r="H174" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="13" t="s">
         <v>202</v>
       </c>
@@ -5270,8 +6323,14 @@
       <c r="F175" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G175" s="15">
+        <v>1</v>
+      </c>
+      <c r="H175" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="13" t="s">
         <v>203</v>
       </c>
@@ -5290,8 +6349,14 @@
       <c r="F176" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G176" s="15">
+        <v>2</v>
+      </c>
+      <c r="H176" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="13" t="s">
         <v>204</v>
       </c>
@@ -5310,8 +6375,14 @@
       <c r="F177" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G177" s="15">
+        <v>2</v>
+      </c>
+      <c r="H177" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="13" t="s">
         <v>205</v>
       </c>
@@ -5330,8 +6401,14 @@
       <c r="F178" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G178" s="15">
+        <v>2</v>
+      </c>
+      <c r="H178" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="13" t="s">
         <v>206</v>
       </c>
@@ -5350,8 +6427,14 @@
       <c r="F179" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G179" s="15">
+        <v>2</v>
+      </c>
+      <c r="H179" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="13" t="s">
         <v>207</v>
       </c>
@@ -5370,8 +6453,14 @@
       <c r="F180" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G180" s="15">
+        <v>2</v>
+      </c>
+      <c r="H180" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="13" t="s">
         <v>208</v>
       </c>
@@ -5389,6 +6478,12 @@
       </c>
       <c r="F181" s="3">
         <v>0</v>
+      </c>
+      <c r="G181" s="15">
+        <v>1</v>
+      </c>
+      <c r="H181" s="11">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
@@ -9587,10 +10682,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J181"/>
+  <dimension ref="A1:K181"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:J1"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9604,7 +10699,7 @@
     <col min="8" max="8" width="8.28515625" style="4" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" style="4" customWidth="1"/>
     <col min="10" max="10" width="8.28515625" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -15408,7 +16503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added ventilation properties to building archetypes
</commit_message>
<xml_diff>
--- a/cea/db/Archetypes/Switzerland/Archetypes_properties.xlsx
+++ b/cea/db/Archetypes/Switzerland/Archetypes_properties.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3732" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3733" uniqueCount="276">
   <si>
     <t>Code</t>
   </si>
@@ -850,6 +850,9 @@
   </si>
   <si>
     <t>win_op</t>
+  </si>
+  <si>
+    <t>f_cros</t>
   </si>
 </sst>
 </file>
@@ -1751,10 +1754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H181"/>
+  <dimension ref="A1:I181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I146" sqref="I146:I181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1764,11 +1767,11 @@
     <col min="3" max="3" width="12.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="4" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="9" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1793,8 +1796,11 @@
       <c r="H1" s="13" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -1819,8 +1825,11 @@
       <c r="H2" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>30</v>
       </c>
@@ -1845,8 +1854,11 @@
       <c r="H3" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>31</v>
       </c>
@@ -1871,8 +1883,11 @@
       <c r="H4" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>32</v>
       </c>
@@ -1897,8 +1912,11 @@
       <c r="H5" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>33</v>
       </c>
@@ -1923,8 +1941,11 @@
       <c r="H6" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>34</v>
       </c>
@@ -1949,8 +1970,11 @@
       <c r="H7" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>35</v>
       </c>
@@ -1975,8 +1999,11 @@
       <c r="H8" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>36</v>
       </c>
@@ -2001,8 +2028,11 @@
       <c r="H9" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>37</v>
       </c>
@@ -2027,8 +2057,11 @@
       <c r="H10" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>38</v>
       </c>
@@ -2053,8 +2086,11 @@
       <c r="H11" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>39</v>
       </c>
@@ -2079,8 +2115,11 @@
       <c r="H12" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>40</v>
       </c>
@@ -2105,8 +2144,11 @@
       <c r="H13" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>53</v>
       </c>
@@ -2131,8 +2173,11 @@
       <c r="H14" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>54</v>
       </c>
@@ -2157,8 +2202,11 @@
       <c r="H15" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>55</v>
       </c>
@@ -2183,8 +2231,11 @@
       <c r="H16" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>56</v>
       </c>
@@ -2209,8 +2260,11 @@
       <c r="H17" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>57</v>
       </c>
@@ -2235,8 +2289,11 @@
       <c r="H18" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>58</v>
       </c>
@@ -2261,8 +2318,11 @@
       <c r="H19" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>59</v>
       </c>
@@ -2287,8 +2347,11 @@
       <c r="H20" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>60</v>
       </c>
@@ -2313,8 +2376,11 @@
       <c r="H21" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>61</v>
       </c>
@@ -2339,8 +2405,11 @@
       <c r="H22" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>62</v>
       </c>
@@ -2365,8 +2434,11 @@
       <c r="H23" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>63</v>
       </c>
@@ -2391,8 +2463,11 @@
       <c r="H24" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>64</v>
       </c>
@@ -2417,8 +2492,11 @@
       <c r="H25" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>41</v>
       </c>
@@ -2444,8 +2522,11 @@
       <c r="H26" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>42</v>
       </c>
@@ -2471,8 +2552,11 @@
       <c r="H27" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>43</v>
       </c>
@@ -2498,8 +2582,11 @@
       <c r="H28" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>44</v>
       </c>
@@ -2525,8 +2612,11 @@
       <c r="H29" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>45</v>
       </c>
@@ -2552,8 +2642,11 @@
       <c r="H30" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>46</v>
       </c>
@@ -2579,8 +2672,11 @@
       <c r="H31" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>47</v>
       </c>
@@ -2606,8 +2702,11 @@
       <c r="H32" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>48</v>
       </c>
@@ -2633,8 +2732,11 @@
       <c r="H33" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>49</v>
       </c>
@@ -2660,8 +2762,11 @@
       <c r="H34" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>50</v>
       </c>
@@ -2687,8 +2792,11 @@
       <c r="H35" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>51</v>
       </c>
@@ -2714,8 +2822,11 @@
       <c r="H36" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>52</v>
       </c>
@@ -2741,8 +2852,11 @@
       <c r="H37" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>65</v>
       </c>
@@ -2767,8 +2881,11 @@
       <c r="H38" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>66</v>
       </c>
@@ -2793,8 +2910,11 @@
       <c r="H39" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>67</v>
       </c>
@@ -2819,8 +2939,11 @@
       <c r="H40" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>68</v>
       </c>
@@ -2845,8 +2968,11 @@
       <c r="H41" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>69</v>
       </c>
@@ -2871,8 +2997,11 @@
       <c r="H42" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>70</v>
       </c>
@@ -2897,8 +3026,11 @@
       <c r="H43" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>71</v>
       </c>
@@ -2923,8 +3055,11 @@
       <c r="H44" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>72</v>
       </c>
@@ -2949,8 +3084,11 @@
       <c r="H45" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>73</v>
       </c>
@@ -2975,8 +3113,11 @@
       <c r="H46" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>74</v>
       </c>
@@ -3001,8 +3142,11 @@
       <c r="H47" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>75</v>
       </c>
@@ -3027,8 +3171,11 @@
       <c r="H48" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>76</v>
       </c>
@@ -3053,8 +3200,11 @@
       <c r="H49" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>77</v>
       </c>
@@ -3079,8 +3229,11 @@
       <c r="H50" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>78</v>
       </c>
@@ -3105,8 +3258,11 @@
       <c r="H51" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
         <v>79</v>
       </c>
@@ -3131,8 +3287,11 @@
       <c r="H52" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>80</v>
       </c>
@@ -3157,8 +3316,11 @@
       <c r="H53" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>81</v>
       </c>
@@ -3183,8 +3345,11 @@
       <c r="H54" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>82</v>
       </c>
@@ -3209,8 +3374,11 @@
       <c r="H55" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>83</v>
       </c>
@@ -3235,8 +3403,11 @@
       <c r="H56" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>84</v>
       </c>
@@ -3261,8 +3432,11 @@
       <c r="H57" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>85</v>
       </c>
@@ -3287,8 +3461,11 @@
       <c r="H58" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
         <v>86</v>
       </c>
@@ -3313,8 +3490,11 @@
       <c r="H59" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
         <v>87</v>
       </c>
@@ -3339,8 +3519,11 @@
       <c r="H60" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>88</v>
       </c>
@@ -3365,8 +3548,11 @@
       <c r="H61" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>245</v>
       </c>
@@ -3391,8 +3577,11 @@
       <c r="H62" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>246</v>
       </c>
@@ -3417,8 +3606,11 @@
       <c r="H63" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>247</v>
       </c>
@@ -3443,8 +3635,11 @@
       <c r="H64" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
         <v>248</v>
       </c>
@@ -3469,8 +3664,11 @@
       <c r="H65" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>249</v>
       </c>
@@ -3495,8 +3693,11 @@
       <c r="H66" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>250</v>
       </c>
@@ -3521,8 +3722,11 @@
       <c r="H67" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
         <v>251</v>
       </c>
@@ -3547,8 +3751,11 @@
       <c r="H68" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
         <v>252</v>
       </c>
@@ -3573,8 +3780,11 @@
       <c r="H69" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
         <v>253</v>
       </c>
@@ -3599,8 +3809,11 @@
       <c r="H70" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
         <v>254</v>
       </c>
@@ -3625,8 +3838,11 @@
       <c r="H71" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
         <v>255</v>
       </c>
@@ -3651,8 +3867,11 @@
       <c r="H72" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
         <v>256</v>
       </c>
@@ -3677,8 +3896,11 @@
       <c r="H73" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
         <v>101</v>
       </c>
@@ -3703,8 +3925,11 @@
       <c r="H74" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
         <v>102</v>
       </c>
@@ -3729,8 +3954,11 @@
       <c r="H75" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
         <v>103</v>
       </c>
@@ -3755,8 +3983,11 @@
       <c r="H76" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
         <v>104</v>
       </c>
@@ -3781,8 +4012,11 @@
       <c r="H77" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
         <v>105</v>
       </c>
@@ -3807,8 +4041,11 @@
       <c r="H78" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
         <v>106</v>
       </c>
@@ -3833,8 +4070,11 @@
       <c r="H79" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>107</v>
       </c>
@@ -3859,8 +4099,11 @@
       <c r="H80" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
         <v>108</v>
       </c>
@@ -3885,8 +4128,11 @@
       <c r="H81" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
         <v>109</v>
       </c>
@@ -3911,8 +4157,11 @@
       <c r="H82" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
         <v>110</v>
       </c>
@@ -3937,8 +4186,11 @@
       <c r="H83" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
         <v>111</v>
       </c>
@@ -3963,8 +4215,11 @@
       <c r="H84" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
         <v>112</v>
       </c>
@@ -3989,8 +4244,11 @@
       <c r="H85" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
         <v>113</v>
       </c>
@@ -4015,8 +4273,11 @@
       <c r="H86" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>114</v>
       </c>
@@ -4041,8 +4302,11 @@
       <c r="H87" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>115</v>
       </c>
@@ -4067,8 +4331,11 @@
       <c r="H88" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
         <v>116</v>
       </c>
@@ -4093,8 +4360,11 @@
       <c r="H89" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
         <v>117</v>
       </c>
@@ -4119,8 +4389,11 @@
       <c r="H90" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
         <v>118</v>
       </c>
@@ -4145,8 +4418,11 @@
       <c r="H91" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>119</v>
       </c>
@@ -4171,8 +4447,11 @@
       <c r="H92" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
         <v>120</v>
       </c>
@@ -4197,8 +4476,11 @@
       <c r="H93" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
         <v>121</v>
       </c>
@@ -4223,8 +4505,11 @@
       <c r="H94" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
         <v>122</v>
       </c>
@@ -4249,8 +4534,11 @@
       <c r="H95" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
         <v>123</v>
       </c>
@@ -4275,8 +4563,11 @@
       <c r="H96" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
         <v>124</v>
       </c>
@@ -4301,8 +4592,11 @@
       <c r="H97" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
         <v>125</v>
       </c>
@@ -4327,8 +4621,11 @@
       <c r="H98" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
         <v>126</v>
       </c>
@@ -4353,8 +4650,11 @@
       <c r="H99" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
         <v>127</v>
       </c>
@@ -4379,8 +4679,11 @@
       <c r="H100" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
         <v>128</v>
       </c>
@@ -4405,8 +4708,11 @@
       <c r="H101" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
         <v>129</v>
       </c>
@@ -4431,8 +4737,11 @@
       <c r="H102" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I102" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
         <v>130</v>
       </c>
@@ -4457,8 +4766,11 @@
       <c r="H103" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I103" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
         <v>131</v>
       </c>
@@ -4483,8 +4795,11 @@
       <c r="H104" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I104" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
         <v>132</v>
       </c>
@@ -4509,8 +4824,11 @@
       <c r="H105" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I105" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
         <v>133</v>
       </c>
@@ -4535,8 +4853,11 @@
       <c r="H106" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I106" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
         <v>134</v>
       </c>
@@ -4561,8 +4882,11 @@
       <c r="H107" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I107" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
         <v>135</v>
       </c>
@@ -4587,8 +4911,11 @@
       <c r="H108" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I108" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
         <v>136</v>
       </c>
@@ -4613,8 +4940,11 @@
       <c r="H109" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I109" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="s">
         <v>137</v>
       </c>
@@ -4639,8 +4969,11 @@
       <c r="H110" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I110" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="s">
         <v>138</v>
       </c>
@@ -4665,8 +4998,11 @@
       <c r="H111" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I111" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
         <v>139</v>
       </c>
@@ -4691,8 +5027,11 @@
       <c r="H112" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I112" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
         <v>140</v>
       </c>
@@ -4717,8 +5056,11 @@
       <c r="H113" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I113" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="13" t="s">
         <v>141</v>
       </c>
@@ -4743,8 +5085,11 @@
       <c r="H114" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I114" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="13" t="s">
         <v>142</v>
       </c>
@@ -4769,8 +5114,11 @@
       <c r="H115" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I115" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="13" t="s">
         <v>143</v>
       </c>
@@ -4795,8 +5143,11 @@
       <c r="H116" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I116" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
         <v>144</v>
       </c>
@@ -4821,8 +5172,11 @@
       <c r="H117" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I117" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
         <v>145</v>
       </c>
@@ -4847,8 +5201,11 @@
       <c r="H118" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I118" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
         <v>146</v>
       </c>
@@ -4873,8 +5230,11 @@
       <c r="H119" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I119" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
         <v>147</v>
       </c>
@@ -4899,8 +5259,11 @@
       <c r="H120" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I120" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="s">
         <v>148</v>
       </c>
@@ -4925,8 +5288,11 @@
       <c r="H121" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I121" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="13" t="s">
         <v>149</v>
       </c>
@@ -4951,8 +5317,11 @@
       <c r="H122" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I122" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="13" t="s">
         <v>150</v>
       </c>
@@ -4977,8 +5346,11 @@
       <c r="H123" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I123" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="s">
         <v>151</v>
       </c>
@@ -5003,8 +5375,11 @@
       <c r="H124" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I124" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="13" t="s">
         <v>152</v>
       </c>
@@ -5029,8 +5404,11 @@
       <c r="H125" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I125" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="13" t="s">
         <v>153</v>
       </c>
@@ -5055,8 +5433,11 @@
       <c r="H126" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I126" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="13" t="s">
         <v>154</v>
       </c>
@@ -5081,8 +5462,11 @@
       <c r="H127" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I127" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="13" t="s">
         <v>155</v>
       </c>
@@ -5107,8 +5491,11 @@
       <c r="H128" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I128" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="13" t="s">
         <v>156</v>
       </c>
@@ -5133,8 +5520,11 @@
       <c r="H129" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I129" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="13" t="s">
         <v>157</v>
       </c>
@@ -5159,8 +5549,11 @@
       <c r="H130" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I130" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="13" t="s">
         <v>158</v>
       </c>
@@ -5185,8 +5578,11 @@
       <c r="H131" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I131" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="13" t="s">
         <v>159</v>
       </c>
@@ -5211,8 +5607,11 @@
       <c r="H132" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I132" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
         <v>160</v>
       </c>
@@ -5237,8 +5636,11 @@
       <c r="H133" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I133" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="13" t="s">
         <v>161</v>
       </c>
@@ -5263,8 +5665,11 @@
       <c r="H134" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I134" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="13" t="s">
         <v>162</v>
       </c>
@@ -5289,8 +5694,11 @@
       <c r="H135" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I135" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="13" t="s">
         <v>163</v>
       </c>
@@ -5315,8 +5723,11 @@
       <c r="H136" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I136" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="13" t="s">
         <v>164</v>
       </c>
@@ -5341,8 +5752,11 @@
       <c r="H137" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I137" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="13" t="s">
         <v>165</v>
       </c>
@@ -5367,8 +5781,11 @@
       <c r="H138" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I138" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="13" t="s">
         <v>166</v>
       </c>
@@ -5393,8 +5810,11 @@
       <c r="H139" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I139" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="13" t="s">
         <v>167</v>
       </c>
@@ -5419,8 +5839,11 @@
       <c r="H140" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I140" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="13" t="s">
         <v>168</v>
       </c>
@@ -5445,8 +5868,11 @@
       <c r="H141" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I141" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="13" t="s">
         <v>169</v>
       </c>
@@ -5471,8 +5897,11 @@
       <c r="H142" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I142" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="13" t="s">
         <v>170</v>
       </c>
@@ -5497,8 +5926,11 @@
       <c r="H143" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I143" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="13" t="s">
         <v>171</v>
       </c>
@@ -5523,8 +5955,11 @@
       <c r="H144" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I144" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
         <v>172</v>
       </c>
@@ -5549,8 +5984,11 @@
       <c r="H145" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I145" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="13" t="s">
         <v>173</v>
       </c>
@@ -5575,8 +6013,11 @@
       <c r="H146" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I146" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="13" t="s">
         <v>174</v>
       </c>
@@ -5601,8 +6042,11 @@
       <c r="H147" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I147" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="13" t="s">
         <v>175</v>
       </c>
@@ -5627,8 +6071,11 @@
       <c r="H148" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I148" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="13" t="s">
         <v>176</v>
       </c>
@@ -5653,8 +6100,11 @@
       <c r="H149" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I149" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="13" t="s">
         <v>177</v>
       </c>
@@ -5679,8 +6129,11 @@
       <c r="H150" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I150" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="13" t="s">
         <v>178</v>
       </c>
@@ -5705,8 +6158,11 @@
       <c r="H151" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I151" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="13" t="s">
         <v>179</v>
       </c>
@@ -5731,8 +6187,11 @@
       <c r="H152" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I152" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="13" t="s">
         <v>180</v>
       </c>
@@ -5757,8 +6216,11 @@
       <c r="H153" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I153" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="13" t="s">
         <v>181</v>
       </c>
@@ -5783,8 +6245,11 @@
       <c r="H154" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I154" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="13" t="s">
         <v>182</v>
       </c>
@@ -5809,8 +6274,11 @@
       <c r="H155" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I155" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="13" t="s">
         <v>183</v>
       </c>
@@ -5835,8 +6303,11 @@
       <c r="H156" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I156" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="13" t="s">
         <v>184</v>
       </c>
@@ -5861,8 +6332,11 @@
       <c r="H157" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I157" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="13" t="s">
         <v>185</v>
       </c>
@@ -5887,8 +6361,11 @@
       <c r="H158" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I158" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="13" t="s">
         <v>186</v>
       </c>
@@ -5913,8 +6390,11 @@
       <c r="H159" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I159" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="13" t="s">
         <v>187</v>
       </c>
@@ -5939,8 +6419,11 @@
       <c r="H160" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I160" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="13" t="s">
         <v>188</v>
       </c>
@@ -5965,8 +6448,11 @@
       <c r="H161" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I161" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="13" t="s">
         <v>189</v>
       </c>
@@ -5991,8 +6477,11 @@
       <c r="H162" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I162" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="13" t="s">
         <v>190</v>
       </c>
@@ -6017,8 +6506,11 @@
       <c r="H163" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I163" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="13" t="s">
         <v>191</v>
       </c>
@@ -6043,8 +6535,11 @@
       <c r="H164" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I164" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="13" t="s">
         <v>192</v>
       </c>
@@ -6069,8 +6564,11 @@
       <c r="H165" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I165" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="13" t="s">
         <v>193</v>
       </c>
@@ -6095,8 +6593,11 @@
       <c r="H166" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I166" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="13" t="s">
         <v>194</v>
       </c>
@@ -6121,8 +6622,11 @@
       <c r="H167" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I167" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="13" t="s">
         <v>195</v>
       </c>
@@ -6147,8 +6651,11 @@
       <c r="H168" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I168" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="13" t="s">
         <v>196</v>
       </c>
@@ -6173,8 +6680,11 @@
       <c r="H169" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I169" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="13" t="s">
         <v>197</v>
       </c>
@@ -6199,8 +6709,11 @@
       <c r="H170" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I170" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="13" t="s">
         <v>198</v>
       </c>
@@ -6225,8 +6738,11 @@
       <c r="H171" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I171" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="13" t="s">
         <v>199</v>
       </c>
@@ -6251,8 +6767,11 @@
       <c r="H172" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I172" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="13" t="s">
         <v>200</v>
       </c>
@@ -6277,8 +6796,11 @@
       <c r="H173" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I173" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="13" t="s">
         <v>201</v>
       </c>
@@ -6303,8 +6825,11 @@
       <c r="H174" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I174" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="13" t="s">
         <v>202</v>
       </c>
@@ -6329,8 +6854,11 @@
       <c r="H175" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I175" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="13" t="s">
         <v>203</v>
       </c>
@@ -6355,8 +6883,11 @@
       <c r="H176" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I176" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="13" t="s">
         <v>204</v>
       </c>
@@ -6381,8 +6912,11 @@
       <c r="H177" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I177" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="13" t="s">
         <v>205</v>
       </c>
@@ -6407,8 +6941,11 @@
       <c r="H178" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I178" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="13" t="s">
         <v>206</v>
       </c>
@@ -6433,8 +6970,11 @@
       <c r="H179" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I179" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="13" t="s">
         <v>207</v>
       </c>
@@ -6459,8 +6999,11 @@
       <c r="H180" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I180" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="13" t="s">
         <v>208</v>
       </c>
@@ -6484,6 +7027,9 @@
       </c>
       <c r="H181" s="11">
         <v>0.9</v>
+      </c>
+      <c r="I181" s="10">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update ventilation properties in archetypes db
</commit_message>
<xml_diff>
--- a/cea/db/Archetypes/Switzerland/Archetypes_properties.xlsx
+++ b/cea/db/Archetypes/Switzerland/Archetypes_properties.xlsx
@@ -1757,7 +1757,7 @@
   <dimension ref="A1:I181"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I146" sqref="I146:I181"/>
+      <selection activeCell="H26" sqref="H26:H181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2520,7 +2520,7 @@
         <v>6</v>
       </c>
       <c r="H26" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I26" s="10">
         <v>0</v>
@@ -2550,7 +2550,7 @@
         <v>6</v>
       </c>
       <c r="H27" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I27" s="10">
         <v>0</v>
@@ -2580,7 +2580,7 @@
         <v>6</v>
       </c>
       <c r="H28" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I28" s="10">
         <v>0</v>
@@ -2610,7 +2610,7 @@
         <v>4</v>
       </c>
       <c r="H29" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I29" s="10">
         <v>0</v>
@@ -2640,7 +2640,7 @@
         <v>2</v>
       </c>
       <c r="H30" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I30" s="10">
         <v>0</v>
@@ -2670,7 +2670,7 @@
         <v>1</v>
       </c>
       <c r="H31" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I31" s="10">
         <v>0</v>
@@ -2700,7 +2700,7 @@
         <v>2</v>
       </c>
       <c r="H32" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I32" s="10">
         <v>0</v>
@@ -2730,7 +2730,7 @@
         <v>2</v>
       </c>
       <c r="H33" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I33" s="10">
         <v>0</v>
@@ -2760,7 +2760,7 @@
         <v>2</v>
       </c>
       <c r="H34" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I34" s="10">
         <v>0</v>
@@ -2790,7 +2790,7 @@
         <v>2</v>
       </c>
       <c r="H35" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I35" s="10">
         <v>0</v>
@@ -2820,7 +2820,7 @@
         <v>2</v>
       </c>
       <c r="H36" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I36" s="10">
         <v>0</v>
@@ -2850,7 +2850,7 @@
         <v>1</v>
       </c>
       <c r="H37" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I37" s="10">
         <v>0</v>
@@ -2879,7 +2879,7 @@
         <v>6</v>
       </c>
       <c r="H38" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I38" s="10">
         <v>0</v>
@@ -2908,7 +2908,7 @@
         <v>6</v>
       </c>
       <c r="H39" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I39" s="10">
         <v>0</v>
@@ -2937,7 +2937,7 @@
         <v>6</v>
       </c>
       <c r="H40" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I40" s="10">
         <v>0</v>
@@ -2966,7 +2966,7 @@
         <v>6</v>
       </c>
       <c r="H41" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I41" s="10">
         <v>0</v>
@@ -2995,7 +2995,7 @@
         <v>2</v>
       </c>
       <c r="H42" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I42" s="10">
         <v>0</v>
@@ -3024,7 +3024,7 @@
         <v>1</v>
       </c>
       <c r="H43" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I43" s="10">
         <v>0</v>
@@ -3053,7 +3053,7 @@
         <v>2</v>
       </c>
       <c r="H44" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I44" s="10">
         <v>0</v>
@@ -3082,7 +3082,7 @@
         <v>2</v>
       </c>
       <c r="H45" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I45" s="10">
         <v>0</v>
@@ -3111,7 +3111,7 @@
         <v>2</v>
       </c>
       <c r="H46" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I46" s="10">
         <v>0</v>
@@ -3140,7 +3140,7 @@
         <v>2</v>
       </c>
       <c r="H47" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I47" s="10">
         <v>0</v>
@@ -3169,7 +3169,7 @@
         <v>2</v>
       </c>
       <c r="H48" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I48" s="10">
         <v>0</v>
@@ -3198,7 +3198,7 @@
         <v>1</v>
       </c>
       <c r="H49" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I49" s="10">
         <v>0</v>
@@ -3227,7 +3227,7 @@
         <v>6</v>
       </c>
       <c r="H50" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I50" s="10">
         <v>1</v>
@@ -3256,7 +3256,7 @@
         <v>6</v>
       </c>
       <c r="H51" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I51" s="10">
         <v>1</v>
@@ -3285,7 +3285,7 @@
         <v>6</v>
       </c>
       <c r="H52" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I52" s="10">
         <v>1</v>
@@ -3314,7 +3314,7 @@
         <v>6</v>
       </c>
       <c r="H53" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I53" s="10">
         <v>1</v>
@@ -3343,7 +3343,7 @@
         <v>2</v>
       </c>
       <c r="H54" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I54" s="10">
         <v>1</v>
@@ -3372,7 +3372,7 @@
         <v>1</v>
       </c>
       <c r="H55" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I55" s="10">
         <v>1</v>
@@ -3401,7 +3401,7 @@
         <v>2</v>
       </c>
       <c r="H56" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I56" s="10">
         <v>1</v>
@@ -3430,7 +3430,7 @@
         <v>2</v>
       </c>
       <c r="H57" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I57" s="10">
         <v>1</v>
@@ -3459,7 +3459,7 @@
         <v>2</v>
       </c>
       <c r="H58" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I58" s="10">
         <v>1</v>
@@ -3488,7 +3488,7 @@
         <v>2</v>
       </c>
       <c r="H59" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I59" s="10">
         <v>1</v>
@@ -3517,7 +3517,7 @@
         <v>2</v>
       </c>
       <c r="H60" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I60" s="10">
         <v>1</v>
@@ -3546,7 +3546,7 @@
         <v>1</v>
       </c>
       <c r="H61" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I61" s="10">
         <v>1</v>
@@ -3575,7 +3575,7 @@
         <v>6</v>
       </c>
       <c r="H62" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I62" s="10">
         <v>1</v>
@@ -3604,7 +3604,7 @@
         <v>6</v>
       </c>
       <c r="H63" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I63" s="10">
         <v>1</v>
@@ -3633,7 +3633,7 @@
         <v>6</v>
       </c>
       <c r="H64" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I64" s="10">
         <v>1</v>
@@ -3662,7 +3662,7 @@
         <v>6</v>
       </c>
       <c r="H65" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I65" s="10">
         <v>1</v>
@@ -3691,7 +3691,7 @@
         <v>2</v>
       </c>
       <c r="H66" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I66" s="10">
         <v>1</v>
@@ -3720,7 +3720,7 @@
         <v>1</v>
       </c>
       <c r="H67" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I67" s="10">
         <v>1</v>
@@ -3749,7 +3749,7 @@
         <v>2</v>
       </c>
       <c r="H68" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I68" s="10">
         <v>1</v>
@@ -3778,7 +3778,7 @@
         <v>2</v>
       </c>
       <c r="H69" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I69" s="10">
         <v>1</v>
@@ -3807,7 +3807,7 @@
         <v>2</v>
       </c>
       <c r="H70" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I70" s="10">
         <v>1</v>
@@ -3836,7 +3836,7 @@
         <v>2</v>
       </c>
       <c r="H71" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I71" s="10">
         <v>1</v>
@@ -3865,7 +3865,7 @@
         <v>2</v>
       </c>
       <c r="H72" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I72" s="10">
         <v>1</v>
@@ -3894,7 +3894,7 @@
         <v>1</v>
       </c>
       <c r="H73" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I73" s="10">
         <v>1</v>
@@ -3923,7 +3923,7 @@
         <v>6</v>
       </c>
       <c r="H74" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I74" s="10">
         <v>0</v>
@@ -3952,7 +3952,7 @@
         <v>6</v>
       </c>
       <c r="H75" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I75" s="10">
         <v>0</v>
@@ -3981,7 +3981,7 @@
         <v>6</v>
       </c>
       <c r="H76" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I76" s="10">
         <v>0</v>
@@ -4010,7 +4010,7 @@
         <v>6</v>
       </c>
       <c r="H77" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I77" s="10">
         <v>0</v>
@@ -4039,7 +4039,7 @@
         <v>2</v>
       </c>
       <c r="H78" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I78" s="10">
         <v>0</v>
@@ -4068,7 +4068,7 @@
         <v>1</v>
       </c>
       <c r="H79" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I79" s="10">
         <v>0</v>
@@ -4097,7 +4097,7 @@
         <v>2</v>
       </c>
       <c r="H80" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I80" s="10">
         <v>0</v>
@@ -4126,7 +4126,7 @@
         <v>2</v>
       </c>
       <c r="H81" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I81" s="10">
         <v>0</v>
@@ -4155,7 +4155,7 @@
         <v>2</v>
       </c>
       <c r="H82" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I82" s="10">
         <v>0</v>
@@ -4184,7 +4184,7 @@
         <v>2</v>
       </c>
       <c r="H83" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I83" s="10">
         <v>0</v>
@@ -4213,7 +4213,7 @@
         <v>2</v>
       </c>
       <c r="H84" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I84" s="10">
         <v>0</v>
@@ -4242,7 +4242,7 @@
         <v>1</v>
       </c>
       <c r="H85" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I85" s="10">
         <v>0</v>
@@ -4271,7 +4271,7 @@
         <v>6</v>
       </c>
       <c r="H86" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I86" s="10">
         <v>0</v>
@@ -4300,7 +4300,7 @@
         <v>6</v>
       </c>
       <c r="H87" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I87" s="10">
         <v>0</v>
@@ -4329,7 +4329,7 @@
         <v>6</v>
       </c>
       <c r="H88" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I88" s="10">
         <v>0</v>
@@ -4358,7 +4358,7 @@
         <v>4</v>
       </c>
       <c r="H89" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I89" s="10">
         <v>0</v>
@@ -4387,7 +4387,7 @@
         <v>2</v>
       </c>
       <c r="H90" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I90" s="10">
         <v>0</v>
@@ -4416,7 +4416,7 @@
         <v>1</v>
       </c>
       <c r="H91" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I91" s="10">
         <v>0</v>
@@ -4445,7 +4445,7 @@
         <v>2</v>
       </c>
       <c r="H92" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I92" s="10">
         <v>0</v>
@@ -4474,7 +4474,7 @@
         <v>2</v>
       </c>
       <c r="H93" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I93" s="10">
         <v>0</v>
@@ -4503,7 +4503,7 @@
         <v>2</v>
       </c>
       <c r="H94" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I94" s="10">
         <v>0</v>
@@ -4532,7 +4532,7 @@
         <v>2</v>
       </c>
       <c r="H95" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I95" s="10">
         <v>0</v>
@@ -4561,7 +4561,7 @@
         <v>2</v>
       </c>
       <c r="H96" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I96" s="10">
         <v>0</v>
@@ -4590,7 +4590,7 @@
         <v>1</v>
       </c>
       <c r="H97" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I97" s="10">
         <v>0</v>
@@ -4619,7 +4619,7 @@
         <v>6</v>
       </c>
       <c r="H98" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I98" s="10">
         <v>1</v>
@@ -4648,7 +4648,7 @@
         <v>6</v>
       </c>
       <c r="H99" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I99" s="10">
         <v>1</v>
@@ -4677,7 +4677,7 @@
         <v>6</v>
       </c>
       <c r="H100" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I100" s="10">
         <v>1</v>
@@ -4706,7 +4706,7 @@
         <v>4</v>
       </c>
       <c r="H101" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I101" s="10">
         <v>1</v>
@@ -4735,7 +4735,7 @@
         <v>2</v>
       </c>
       <c r="H102" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I102" s="10">
         <v>1</v>
@@ -4764,7 +4764,7 @@
         <v>1</v>
       </c>
       <c r="H103" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I103" s="10">
         <v>1</v>
@@ -4793,7 +4793,7 @@
         <v>2</v>
       </c>
       <c r="H104" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I104" s="10">
         <v>1</v>
@@ -4822,7 +4822,7 @@
         <v>2</v>
       </c>
       <c r="H105" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I105" s="10">
         <v>1</v>
@@ -4851,7 +4851,7 @@
         <v>2</v>
       </c>
       <c r="H106" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I106" s="10">
         <v>1</v>
@@ -4880,7 +4880,7 @@
         <v>2</v>
       </c>
       <c r="H107" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I107" s="10">
         <v>1</v>
@@ -4909,7 +4909,7 @@
         <v>2</v>
       </c>
       <c r="H108" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I108" s="10">
         <v>1</v>
@@ -4938,7 +4938,7 @@
         <v>1</v>
       </c>
       <c r="H109" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I109" s="10">
         <v>1</v>
@@ -4967,7 +4967,7 @@
         <v>6</v>
       </c>
       <c r="H110" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I110" s="10">
         <v>0</v>
@@ -4996,7 +4996,7 @@
         <v>6</v>
       </c>
       <c r="H111" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I111" s="10">
         <v>0</v>
@@ -5025,7 +5025,7 @@
         <v>6</v>
       </c>
       <c r="H112" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I112" s="10">
         <v>0</v>
@@ -5054,7 +5054,7 @@
         <v>4</v>
       </c>
       <c r="H113" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I113" s="10">
         <v>0</v>
@@ -5083,7 +5083,7 @@
         <v>2</v>
       </c>
       <c r="H114" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I114" s="10">
         <v>0</v>
@@ -5112,7 +5112,7 @@
         <v>1</v>
       </c>
       <c r="H115" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I115" s="10">
         <v>0</v>
@@ -5141,7 +5141,7 @@
         <v>2</v>
       </c>
       <c r="H116" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I116" s="10">
         <v>0</v>
@@ -5170,7 +5170,7 @@
         <v>2</v>
       </c>
       <c r="H117" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I117" s="10">
         <v>0</v>
@@ -5199,7 +5199,7 @@
         <v>2</v>
       </c>
       <c r="H118" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I118" s="10">
         <v>0</v>
@@ -5228,7 +5228,7 @@
         <v>2</v>
       </c>
       <c r="H119" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I119" s="10">
         <v>0</v>
@@ -5257,7 +5257,7 @@
         <v>2</v>
       </c>
       <c r="H120" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I120" s="10">
         <v>0</v>
@@ -5286,7 +5286,7 @@
         <v>1</v>
       </c>
       <c r="H121" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I121" s="10">
         <v>0</v>
@@ -5315,7 +5315,7 @@
         <v>6</v>
       </c>
       <c r="H122" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I122" s="10">
         <v>1</v>
@@ -5344,7 +5344,7 @@
         <v>6</v>
       </c>
       <c r="H123" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I123" s="10">
         <v>1</v>
@@ -5373,7 +5373,7 @@
         <v>6</v>
       </c>
       <c r="H124" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I124" s="10">
         <v>1</v>
@@ -5402,7 +5402,7 @@
         <v>4</v>
       </c>
       <c r="H125" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I125" s="10">
         <v>1</v>
@@ -5431,7 +5431,7 @@
         <v>2</v>
       </c>
       <c r="H126" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I126" s="10">
         <v>1</v>
@@ -5460,7 +5460,7 @@
         <v>1</v>
       </c>
       <c r="H127" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I127" s="10">
         <v>1</v>
@@ -5489,7 +5489,7 @@
         <v>2</v>
       </c>
       <c r="H128" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I128" s="10">
         <v>1</v>
@@ -5518,7 +5518,7 @@
         <v>2</v>
       </c>
       <c r="H129" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I129" s="10">
         <v>1</v>
@@ -5547,7 +5547,7 @@
         <v>2</v>
       </c>
       <c r="H130" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I130" s="10">
         <v>1</v>
@@ -5576,7 +5576,7 @@
         <v>2</v>
       </c>
       <c r="H131" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I131" s="10">
         <v>1</v>
@@ -5605,7 +5605,7 @@
         <v>2</v>
       </c>
       <c r="H132" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I132" s="10">
         <v>1</v>
@@ -5634,7 +5634,7 @@
         <v>1</v>
       </c>
       <c r="H133" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I133" s="10">
         <v>1</v>
@@ -5663,7 +5663,7 @@
         <v>6</v>
       </c>
       <c r="H134" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I134" s="10">
         <v>1</v>
@@ -5692,7 +5692,7 @@
         <v>6</v>
       </c>
       <c r="H135" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I135" s="10">
         <v>1</v>
@@ -5721,7 +5721,7 @@
         <v>6</v>
       </c>
       <c r="H136" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I136" s="10">
         <v>1</v>
@@ -5750,7 +5750,7 @@
         <v>4</v>
       </c>
       <c r="H137" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I137" s="10">
         <v>1</v>
@@ -5779,7 +5779,7 @@
         <v>2</v>
       </c>
       <c r="H138" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I138" s="10">
         <v>1</v>
@@ -5808,7 +5808,7 @@
         <v>1</v>
       </c>
       <c r="H139" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I139" s="10">
         <v>1</v>
@@ -5837,7 +5837,7 @@
         <v>2</v>
       </c>
       <c r="H140" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I140" s="10">
         <v>1</v>
@@ -5866,7 +5866,7 @@
         <v>2</v>
       </c>
       <c r="H141" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I141" s="10">
         <v>1</v>
@@ -5895,7 +5895,7 @@
         <v>2</v>
       </c>
       <c r="H142" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I142" s="10">
         <v>1</v>
@@ -5924,7 +5924,7 @@
         <v>2</v>
       </c>
       <c r="H143" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I143" s="10">
         <v>1</v>
@@ -5953,7 +5953,7 @@
         <v>2</v>
       </c>
       <c r="H144" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I144" s="10">
         <v>1</v>
@@ -5982,7 +5982,7 @@
         <v>1</v>
       </c>
       <c r="H145" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I145" s="10">
         <v>1</v>
@@ -6011,7 +6011,7 @@
         <v>6</v>
       </c>
       <c r="H146" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I146" s="10">
         <v>0</v>
@@ -6040,7 +6040,7 @@
         <v>6</v>
       </c>
       <c r="H147" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I147" s="10">
         <v>0</v>
@@ -6069,7 +6069,7 @@
         <v>6</v>
       </c>
       <c r="H148" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I148" s="10">
         <v>0</v>
@@ -6098,7 +6098,7 @@
         <v>4</v>
       </c>
       <c r="H149" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I149" s="10">
         <v>0</v>
@@ -6127,7 +6127,7 @@
         <v>2</v>
       </c>
       <c r="H150" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I150" s="10">
         <v>0</v>
@@ -6156,7 +6156,7 @@
         <v>1</v>
       </c>
       <c r="H151" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I151" s="10">
         <v>0</v>
@@ -6185,7 +6185,7 @@
         <v>2</v>
       </c>
       <c r="H152" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I152" s="10">
         <v>0</v>
@@ -6214,7 +6214,7 @@
         <v>2</v>
       </c>
       <c r="H153" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I153" s="10">
         <v>0</v>
@@ -6243,7 +6243,7 @@
         <v>2</v>
       </c>
       <c r="H154" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I154" s="10">
         <v>0</v>
@@ -6272,7 +6272,7 @@
         <v>2</v>
       </c>
       <c r="H155" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I155" s="10">
         <v>0</v>
@@ -6301,7 +6301,7 @@
         <v>2</v>
       </c>
       <c r="H156" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I156" s="10">
         <v>0</v>
@@ -6330,7 +6330,7 @@
         <v>1</v>
       </c>
       <c r="H157" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I157" s="10">
         <v>0</v>
@@ -6359,7 +6359,7 @@
         <v>6</v>
       </c>
       <c r="H158" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I158" s="10">
         <v>0</v>
@@ -6388,7 +6388,7 @@
         <v>6</v>
       </c>
       <c r="H159" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I159" s="10">
         <v>0</v>
@@ -6417,7 +6417,7 @@
         <v>6</v>
       </c>
       <c r="H160" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I160" s="10">
         <v>0</v>
@@ -6446,7 +6446,7 @@
         <v>6</v>
       </c>
       <c r="H161" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I161" s="10">
         <v>0</v>
@@ -6475,7 +6475,7 @@
         <v>2</v>
       </c>
       <c r="H162" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I162" s="10">
         <v>0</v>
@@ -6504,7 +6504,7 @@
         <v>1</v>
       </c>
       <c r="H163" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I163" s="10">
         <v>0</v>
@@ -6533,7 +6533,7 @@
         <v>2</v>
       </c>
       <c r="H164" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I164" s="10">
         <v>0</v>
@@ -6562,7 +6562,7 @@
         <v>2</v>
       </c>
       <c r="H165" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I165" s="10">
         <v>0</v>
@@ -6591,7 +6591,7 @@
         <v>2</v>
       </c>
       <c r="H166" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I166" s="10">
         <v>0</v>
@@ -6620,7 +6620,7 @@
         <v>2</v>
       </c>
       <c r="H167" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I167" s="10">
         <v>0</v>
@@ -6649,7 +6649,7 @@
         <v>2</v>
       </c>
       <c r="H168" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I168" s="10">
         <v>0</v>
@@ -6678,7 +6678,7 @@
         <v>1</v>
       </c>
       <c r="H169" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I169" s="10">
         <v>0</v>
@@ -6707,7 +6707,7 @@
         <v>6</v>
       </c>
       <c r="H170" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I170" s="10">
         <v>0</v>
@@ -6736,7 +6736,7 @@
         <v>6</v>
       </c>
       <c r="H171" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I171" s="10">
         <v>0</v>
@@ -6765,7 +6765,7 @@
         <v>6</v>
       </c>
       <c r="H172" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I172" s="10">
         <v>0</v>
@@ -6794,7 +6794,7 @@
         <v>4</v>
       </c>
       <c r="H173" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I173" s="10">
         <v>0</v>
@@ -6823,7 +6823,7 @@
         <v>2</v>
       </c>
       <c r="H174" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I174" s="10">
         <v>0</v>
@@ -6852,7 +6852,7 @@
         <v>1</v>
       </c>
       <c r="H175" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I175" s="10">
         <v>0</v>
@@ -6881,7 +6881,7 @@
         <v>2</v>
       </c>
       <c r="H176" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I176" s="10">
         <v>0</v>
@@ -6910,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="H177" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I177" s="10">
         <v>0</v>
@@ -6939,7 +6939,7 @@
         <v>2</v>
       </c>
       <c r="H178" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I178" s="10">
         <v>0</v>
@@ -6968,7 +6968,7 @@
         <v>2</v>
       </c>
       <c r="H179" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I179" s="10">
         <v>0</v>
@@ -6997,7 +6997,7 @@
         <v>2</v>
       </c>
       <c r="H180" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I180" s="10">
         <v>0</v>
@@ -7026,7 +7026,7 @@
         <v>1</v>
       </c>
       <c r="H181" s="11">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I181" s="10">
         <v>0</v>

</xml_diff>